<commit_message>
update kế hoạch dự phòng
</commit_message>
<xml_diff>
--- a/doc/KHDUPHONG.xlsx
+++ b/doc/KHDUPHONG.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="149">
   <si>
     <t>KẾ HOẠCH THỰC HIỆN KHÓA LUẬN TỐT NGHIỆP</t>
   </si>
@@ -571,6 +571,18 @@
 - Tiến hành code front-end các component cho chức năng thêm, xóa sửa kỹ năng kỹ thuật, ngoại ngữ.</t>
   </si>
   <si>
+    <t>Nghỉ Tết Nguyên Đán, tìm hiểu thêm về back-end:
+- Củng cố kiến thức về Spring Boot(Spring Security, Spring Data), Hibernate.
+- Tìm hiểu cách thiết lập quan hệ giữa các bảng trong SQL để tối ưu việc tìm kiếm.
+- Tìm hiểu java template engine thymeleaf.</t>
+  </si>
+  <si>
+    <t>Nghỉ Tết Nguyên Đán, tìm hiểu thêm về back-end:
+- Củng cố kiến thức về Spring Boot(Spring Security, Spring Data), Hibernate.
+- Tìm hiểu cách thiết lập quan hệ giữa các bảng trong SQL để tối ưu việc tìm kiếm.
+- Tìm hiểu  java template engine thymeleaf.</t>
+  </si>
+  <si>
     <t>- Tìm hiểu các dependency Spring Boot (tài liệu Fsoft cung cấp, spring.io):
 + spring-boot-starter-web
 + spring-boot-starter-data-jpa
@@ -581,28 +593,69 @@
 - Viết User stories với các actor:
 + Nhân viên (Quản lý kỹ năng CV, Tìm kiếm cơ bản, Đánh giá, Hướng dẫn sử dụng)
 + Quản lý(Tìm kiếm nâng cao,Đánh giá, Xem đánh giá).
-+ Nhân sự (Tìm kiếm nâng cao, Xác nhận CV, Cập nhật thông tin nhân viên, Phân tích dữ liệu mạng xã hội của nhân viên).B12
++ Nhân sự (Tìm kiếm nâng cao, Xác nhận CV, Cập nhật thông tin nhân viên, Phân tích dữ liệu mạng xã hội của nhân viên).
 - Chỉnh sửa yêu cấu đề tài (nghiệp vụ tuyển dụng)</t>
-  </si>
-  <si>
-    <t>Nghỉ Tết Nguyên Đán, tìm hiểu thêm về back-end:
-- Củng cố kiến thức về Spring Boot(Spring Security, Spring Data), Hibernate.
-- Tìm hiểu cách thiết lập quan hệ giữa các bảng trong SQL để tối ưu việc tìm kiếm.
-- Tìm hiểu java template engine thymeleaf.</t>
-  </si>
-  <si>
-    <t>Nghỉ Tết Nguyên Đán, tìm hiểu thêm về back-end:
-- Củng cố kiến thức về Spring Boot(Spring Security, Spring Data), Hibernate.
-- Tìm hiểu cách thiết lập quan hệ giữa các bảng trong SQL để tối ưu việc tìm kiếm.
-- Tìm hiểu  java template engine thymeleaf.</t>
   </si>
   <si>
     <t>- Thiết kế Usecase, đặc tả.
 - Thiết kế Entity diagram.
 - Thiết lập các quan hệ entity trên hibernate
 - Tạo api spring boot nhân viên, bằng cấp, chứng chỉ
-- Tạo trang về bằng cấp, chứng chỉ
-- Tích hợp Angular vào Spring-boot</t>
+- Tạo trang quản lý bằng cấp, chứng chỉ</t>
+  </si>
+  <si>
+    <t>- Chỉnh sửa lại Thiết kế Usecase, đặc tả, Sitemap, Entity diagram.
+- Điều chỉnh requirentment
+- Tạo api về kỹ năng, học vấn.
+- Tạo các trang quản lý kỹ năng, học vấn.</t>
+  </si>
+  <si>
+    <t>- Chỉnh sửa lại Thiết kế Usecase, đặc tả,  Sitemap, Entity, Activity, Sequency, Class diagram.
+- Tạo api về kinh nghiệm làm việc, thông tin cá nhân.
+- Tạo trang quản lý kinh nghiệm làm việc, thông tin cá nhân.
+- Thiết kế một số Test Case và Unit Test cho các tính năng trên.</t>
+  </si>
+  <si>
+    <t>- Tạo api cho nhập, xuất dữ liệu nhân viên, tính năng hỗ trợ nhân viên.
+- Tích hợp xác thực tài khoản với CAS
+- Tạo trang cho nhập dữ liệu nhân viên mô phỏng spreadsheet.
+- Deploy phiên bản code v0.1</t>
+  </si>
+  <si>
+    <t>- Điều chỉnh thiết kế màn hình của nhân viên.
+- Test và fix các lổi trong code
+- Viết chức năng logging nhật ký thay đổi.
+- Thiết kế Test Case và Unit Test cho các tính năng trên.
+- Điều chỉnh các trang giao diện và sửa lỗi thymeleaf.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Tạo trang xem nhật ký thay đổi dữ liệu.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>- Phân quyền ứng dụng
+- Viết thuật toán tìm kiếm sắp xếp ứng viên cho dự án.</t>
+    </r>
+  </si>
+  <si>
+    <t>- Thiết kế các màn hình của nhân viên quản lý
+- Tạo api cho chức năng của nhân viên quản lý dự án : quản lý dự án, quản lý vị trí trong dự án, tìm kiếm ứng viên cho dự án.
+- Tạo trang quản lý dự án, vị trí trong dự án và tìm kiếm ứng viên.</t>
+  </si>
+  <si>
+    <t>- Thiết kế các màn hình cho nhân viên nhân sự.
+- Tạo API tính năng duyệt cv cho nhân sự, thống kê, quản lý dữ liệu, thống kê nhân viên.
+- Tạo các trang thống kê, quản lý dữ liệu.
+- Chỉnh sửa Sequence và Class diagram
+- Viết tài liệu kiến thức nền tảng, tổng quan, mục tiêu của đồ án.</t>
+  </si>
+  <si>
+    <t>- Test các tính năng và fix lỗi API, thymeleaf.</t>
   </si>
 </sst>
 </file>
@@ -11155,8 +11208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11482,7 +11535,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="57" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>13</v>
@@ -11554,7 +11607,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>19</v>
@@ -11590,7 +11643,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>22</v>
@@ -11626,7 +11679,7 @@
         <v>6</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>24</v>
@@ -11657,7 +11710,7 @@
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
     </row>
-    <row r="16" spans="1:26" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>7</v>
       </c>
@@ -11698,7 +11751,7 @@
         <v>8</v>
       </c>
       <c r="B17" s="57" t="s">
-        <v>29</v>
+        <v>141</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>30</v>
@@ -11734,7 +11787,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="57" t="s">
-        <v>32</v>
+        <v>142</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>33</v>
@@ -11770,7 +11823,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="57" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>36</v>
@@ -11806,7 +11859,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="57" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>39</v>
@@ -11842,7 +11895,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>41</v>
@@ -11878,7 +11931,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="57" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>44</v>
@@ -11914,7 +11967,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="57" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>46</v>
@@ -11950,7 +12003,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="57" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>48</v>

</xml_diff>